<commit_message>
Add simulation for hospital queue analysis with M/M/1 and M/M/2 models
- Implemented simulation logic in `simulacao.py` to analyze patient queues.
- Created `SimulationConfig` class for loading and saving simulation parameters from/to JSON.
- Developed `QueueingModel` base class and specific models `MM1Model` and `MM2Model`.
- Added metrics calculation for utilization, average queue length, and average wait time.
- Introduced `HospitalQueueAnalyzer` for comparing metrics between different models.
- Generated output files including configuration and metrics in CSV format.
- Added visualization of queue performance comparison using Matplotlib.
- Included command-line interface for flexible simulation configuration.
</commit_message>
<xml_diff>
--- a/projetos/PJ-econometria/Teste de Hipótese no Excel.xlsx
+++ b/projetos/PJ-econometria/Teste de Hipótese no Excel.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/003142078892790f/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\lucas\Github\Public\sandbox-estatistica\projetos\PJ-econometria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{7BA14E16-8B7D-4ED8-B058-A272F8387748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22F1A458-93F8-4100-ADF9-B8636F9FB1F0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DF0F56-EFEC-41E5-BC8D-B0C194DD4F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="15" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{60432254-F301-44F0-845C-6758439D1BE3}"/>
+    <workbookView xWindow="-38520" yWindow="15" windowWidth="38640" windowHeight="15720" activeTab="4" xr2:uid="{60432254-F301-44F0-845C-6758439D1BE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
     <sheet name="Análise de Dados" sheetId="3" r:id="rId2"/>
+    <sheet name="Aluguel" sheetId="4" r:id="rId3"/>
+    <sheet name="Planilha2" sheetId="5" r:id="rId4"/>
+    <sheet name="Planilha3" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Teste 1</t>
   </si>
@@ -116,13 +119,67 @@
   </si>
   <si>
     <t>Variável X 2</t>
+  </si>
+  <si>
+    <t>Imóvel</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>preço</t>
+  </si>
+  <si>
+    <t>ANO</t>
+  </si>
+  <si>
+    <t>PIB (R$)</t>
+  </si>
+  <si>
+    <t>Anova: fator único</t>
+  </si>
+  <si>
+    <t>RESUMO</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Contagem</t>
+  </si>
+  <si>
+    <t>Soma</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Variância</t>
+  </si>
+  <si>
+    <t>Coluna 1</t>
+  </si>
+  <si>
+    <t>Coluna 2</t>
+  </si>
+  <si>
+    <t>Fonte da variação</t>
+  </si>
+  <si>
+    <t>F crítico</t>
+  </si>
+  <si>
+    <t>Entre grupos</t>
+  </si>
+  <si>
+    <t>Dentro dos grupos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +203,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -183,13 +265,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -198,29 +317,132 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -251,6 +473,957 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Aluguel!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>preço</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Aluguel!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Aluguel!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7434-4E72-B44A-A505CA1CCDF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="473121568"/>
+        <c:axId val="473111488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="473121568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="473111488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="473111488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="473121568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -818,14 +1991,67 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>77787</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>112712</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E978E64-325F-E6B5-D01D-44A1AB80DABF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{856A9B86-8BF5-4657-AB88-21B673F4FF23}" name="Tabela1" displayName="Tabela1" ref="A1:D34" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{856A9B86-8BF5-4657-AB88-21B673F4FF23}" name="Tabela1" displayName="Tabela1" ref="A1:D34" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:D34" xr:uid="{856A9B86-8BF5-4657-AB88-21B673F4FF23}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{561B0E9D-9E5D-432C-A90D-648456A58DB2}" name="OBS"/>
     <tableColumn id="2" xr3:uid="{AF28D3AC-8A40-4F36-A308-024EBF5BEC38}" name="Teste 1"/>
     <tableColumn id="3" xr3:uid="{AE5B3F66-411B-48EE-B037-D306015386F5}" name="Teste 2"/>
     <tableColumn id="4" xr3:uid="{6D7CD57E-70E3-4221-BB70-2B9AF1040A12}" name="Y"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87D89A7B-E0E2-49BE-A05D-1A4D09477E92}" name="Tabela2" displayName="Tabela2" ref="A1:C11" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:C11" xr:uid="{87D89A7B-E0E2-49BE-A05D-1A4D09477E92}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{FD5F3416-84AD-46CC-88C6-8B94DB7ABC1A}" name="Imóvel" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{7E047790-021C-498D-B6FB-1F5745D56484}" name="m2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{BC25F255-9993-4243-9ED5-2CA45D4AEEA3}" name="preço" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1632,7 +2858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD63032-1D7E-4113-B05B-D71E3367619E}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1650,7 +2876,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3"/>
@@ -1663,7 +2889,7 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1674,7 +2900,7 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1"/>
@@ -1687,10 +2913,10 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>9.7898841552098062E-2</v>
       </c>
       <c r="C4" s="3"/>
@@ -1702,10 +2928,10 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>9.5841831772428034E-3</v>
       </c>
       <c r="C5" s="3"/>
@@ -1717,10 +2943,10 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>-5.6443537944274348E-2</v>
       </c>
       <c r="C6" s="3"/>
@@ -1732,10 +2958,10 @@
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>2.873928958810847</v>
       </c>
       <c r="C7" s="3"/>
@@ -1747,10 +2973,10 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>33</v>
       </c>
       <c r="C8" s="3"/>
@@ -1762,7 +2988,7 @@
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1773,7 +2999,7 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3"/>
@@ -1786,7 +3012,7 @@
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1807,22 +3033,22 @@
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>2.397788373070199</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>1.1988941865350995</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>0.14515392950794276</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>0.86549290181860505</v>
       </c>
       <c r="G12" s="3"/>
@@ -1830,43 +3056,43 @@
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>30</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>247.78402980874793</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>8.2594676602915982</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>32</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>250.18181818181813</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1877,7 +3103,7 @@
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1904,89 +3130,89 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>4.5021624089606718</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>1.5757949132055473</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>2.8570738306307808</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>7.6952169129695875E-3</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>1.2839598609413829</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>7.7203649569799602</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>1.2839598609413829</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <v>7.7203649569799602</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>5.7750143252347308E-3</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>1.8530913778476491E-2</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>0.31164217772910713</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>0.75746801153400511</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>-3.2070160474640903E-2</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>4.3620189125110363E-2</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <v>-3.2070160474640903E-2</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <v>4.3620189125110363E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>-6.5325009326787512E-3</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>1.8932885941136443E-2</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>-0.34503461083475151</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>0.73247580560703085</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>-4.5198612408554648E-2</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>3.2133610543197147E-2</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="4">
         <v>-4.5198612408554648E-2</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="4">
         <v>3.2133610543197147E-2</v>
       </c>
     </row>
@@ -1994,4 +3220,450 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A58516-FBEA-4EB2-B496-E7A145731F5F}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9">
+        <v>50</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9">
+        <v>75</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9">
+        <v>100</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>120</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>60</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>80</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9">
+        <v>95</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9">
+        <v>110</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9">
+        <v>70</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9">
+        <v>85</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0D0585-55ED-4B8E-B1FB-8C887EDFD960}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="10">
+        <v>2010</v>
+      </c>
+      <c r="B2" s="10">
+        <v>19938.599999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="10">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="10">
+        <v>22259.91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="10">
+        <v>2012</v>
+      </c>
+      <c r="B4" s="10">
+        <v>24278.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="10">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="10">
+        <v>26657.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="10">
+        <v>28648.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="10">
+        <v>29466.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="10">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="10">
+        <v>30558.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="10">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="10">
+        <v>31843.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="10">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="10">
+        <v>33593.82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B11" s="10">
+        <v>35161.699999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="10">
+        <v>35935.69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="10">
+        <v>42247.519999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50214479-7EAC-447B-AEE1-DAEF858EA34F}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="13">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13">
+        <v>24186</v>
+      </c>
+      <c r="D5" s="13">
+        <v>2015.5</v>
+      </c>
+      <c r="E5" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="14">
+        <v>12</v>
+      </c>
+      <c r="C6" s="14">
+        <v>360591.42000000004</v>
+      </c>
+      <c r="D6" s="14">
+        <v>30049.285000000003</v>
+      </c>
+      <c r="E6" s="14">
+        <v>39603299.026499838</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="13">
+        <v>4715358608.5573492</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13">
+        <v>4715358608.5573492</v>
+      </c>
+      <c r="E11" s="13">
+        <v>238.12950822911648</v>
+      </c>
+      <c r="F11" s="13">
+        <v>2.7726158772255549E-13</v>
+      </c>
+      <c r="G11" s="13">
+        <v>4.3009495017776587</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="13">
+        <v>435636432.29149997</v>
+      </c>
+      <c r="C12" s="13">
+        <v>22</v>
+      </c>
+      <c r="D12" s="13">
+        <v>19801656.013249997</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="14">
+        <v>5150995040.8488493</v>
+      </c>
+      <c r="C14" s="14">
+        <v>23</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>